<commit_message>
Update VFLCR_Box.xlsx and Reaadme.txt files.
</commit_message>
<xml_diff>
--- a/VFLCR_Box.xlsx
+++ b/VFLCR_Box.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VFLCRExcelConverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5DC91C-415E-46DB-B1FE-F450FD910BBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F328BA6-F2DF-449D-AEC0-85DECE036B49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="600" windowWidth="25392" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="624" yWindow="336" windowWidth="25392" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VFLCR_Box_X" sheetId="1" r:id="rId1"/>
@@ -4846,12 +4846,13 @@
   <dimension ref="A1:T888"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="15" max="15" width="20" customWidth="1"/>
+    <col min="19" max="19" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -4948,7 +4949,7 @@
         <v>100</v>
       </c>
       <c r="E3">
-        <v>125</v>
+        <v>255</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -5058,10 +5059,12 @@
         <v>100</v>
       </c>
       <c r="D7">
+        <f>D3</f>
         <v>100</v>
       </c>
       <c r="E7">
-        <v>125</v>
+        <f>E3</f>
+        <v>255</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -10648,7 +10651,7 @@
   <dimension ref="A1:T888"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10729,10 +10732,12 @@
         <v>100</v>
       </c>
       <c r="D3">
+        <f>VFLCR_Box_X!D3</f>
         <v>100</v>
       </c>
       <c r="E3">
-        <v>125</v>
+        <f>VFLCR_Box_X!E3</f>
+        <v>255</v>
       </c>
       <c r="H3" s="1">
         <f>P21</f>
@@ -10866,10 +10871,12 @@
         <v>100</v>
       </c>
       <c r="D7">
+        <f>VFLCR_Box_X!D7</f>
         <v>100</v>
       </c>
       <c r="E7">
-        <v>125</v>
+        <f>VFLCR_Box_X!E7</f>
+        <v>255</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>

</xml_diff>